<commit_message>
Back-end finalizado y correcciones Listas de Precios
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\pack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014AE065-8E69-43DB-BA69-4E956D077778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paquete" sheetId="1" r:id="rId1"/>
+    <sheet name="Precios" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="Estudios">Paquete!$C$22:$E$23</definedName>
-    <definedName name="Paquete" localSheetId="0">Paquete!$A$3:$C$16</definedName>
+    <definedName name="Estudios">Precios!$B$15:$E$16</definedName>
+    <definedName name="Precios" localSheetId="0">[1]Precios!$A$3:$C$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Clave</t>
   </si>
@@ -78,36 +82,9 @@
     <t>Activo</t>
   </si>
   <si>
-    <t>Nombre largo</t>
-  </si>
-  <si>
     <t>Área</t>
   </si>
   <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>{{Paquete.Clave}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.NombreLargo}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.Area}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.Departamento}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.Activo}}</t>
-  </si>
-  <si>
-    <t>{{Paquete.visible}}</t>
-  </si>
-  <si>
     <t>Estudios</t>
   </si>
   <si>
@@ -121,12 +98,30 @@
   </si>
   <si>
     <t>Visible</t>
+  </si>
+  <si>
+    <t>{{Precios.Clave}}</t>
+  </si>
+  <si>
+    <t>{{Precios.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Precios.Activo}}</t>
+  </si>
+  <si>
+    <t>{{Precios.visible}}</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>{{item.Precio}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,14 +202,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -286,6 +281,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Precios"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,11 +592,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,11 +605,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -610,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="1"/>
@@ -627,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="1"/>
@@ -641,10 +649,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="1"/>
@@ -658,10 +666,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
@@ -674,12 +682,8 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="1"/>
       <c r="E11" s="8"/>
@@ -691,31 +695,44 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="8"/>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,41 +752,15 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="14">
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E5:F5"/>
@@ -777,15 +768,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio area a string
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014AE065-8E69-43DB-BA69-4E956D077778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05ECAB-48C1-4064-897F-943CAD983AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,20 +109,20 @@
     <t>{{Precios.Activo}}</t>
   </si>
   <si>
-    <t>{{Precios.visible}}</t>
-  </si>
-  <si>
     <t>Precio</t>
   </si>
   <si>
     <t>{{item.Precio}}</t>
+  </si>
+  <si>
+    <t>{{Precios.Visibilidad}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +161,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -202,14 +211,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +608,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,11 +617,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -644,7 +656,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -669,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
@@ -695,11 +707,11 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -712,7 +724,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -726,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,11 +766,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:C1"/>
@@ -768,6 +775,11 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
bug  parametros cambios de unidades
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB05ECAB-48C1-4064-897F-943CAD983AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Precios" sheetId="1" r:id="rId1"/>
@@ -19,8 +18,11 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="Compañias">Precios!$AB$15:$AG$16</definedName>
     <definedName name="Estudios">Precios!$B$15:$E$16</definedName>
+    <definedName name="Medicos">Precios!$T$15:$Y$16</definedName>
     <definedName name="Precios" localSheetId="0">[1]Precios!$A$3:$C$16</definedName>
+    <definedName name="Sucursales">Precios!$J$15:$O$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Clave</t>
   </si>
@@ -117,12 +119,27 @@
   <si>
     <t>{{Precios.Visibilidad}}</t>
   </si>
+  <si>
+    <t>Sucursales</t>
+  </si>
+  <si>
+    <t>Médicos</t>
+  </si>
+  <si>
+    <t>Compañias</t>
+  </si>
+  <si>
+    <t>Lista de Precios</t>
+  </si>
+  <si>
+    <t>{{item.ListaPrecio}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +187,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -211,6 +236,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -220,9 +251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,11 +634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,104 +646,128 @@
     <col min="1" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:33" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="J13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="T13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="AB13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>0</v>
       </c>
@@ -726,8 +780,44 @@
       <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="T14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y14" s="8"/>
+      <c r="AB14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG14" s="8"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -740,32 +830,89 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="12"/>
+      <c r="T15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y15" s="12"/>
+      <c r="AB15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG15" s="12"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="35">
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:C1"/>
@@ -780,6 +927,27 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="AB13:AG13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="T13:Y13"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:Y14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:Y16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ListPriceForm excel format condition
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/PriceList/ListadePrecioFormulario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.Catalog\wwwroot\layout\excel\PriceList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87364CF6-69A9-4D9E-8FC4-9FB68BBFAFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBE8718-71FD-4617-AC15-86CDDBCFCE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Precios" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Sucursales" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Compañias">Compañias!$A$4:$F$5</definedName>
+    <definedName name="Compañias">Compañias!$A$4:$C$5</definedName>
     <definedName name="Estudios">Estudios!$A$4:$D$5</definedName>
     <definedName name="Paquetes">Paquetes!$A$4:$D$5</definedName>
-    <definedName name="Sucursales">Sucursales!$B$4:$D$5</definedName>
+    <definedName name="Sucursales">Sucursales!$A$4:$C$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -245,24 +245,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -629,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB13" sqref="AB13:AG15"/>
     </sheetView>
   </sheetViews>
@@ -643,11 +700,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -655,13 +712,13 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -672,13 +729,13 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -689,13 +746,13 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -706,13 +763,13 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -721,11 +778,11 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -733,27 +790,27 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
@@ -763,23 +820,23 @@
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
@@ -788,8 +845,8 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
@@ -798,6 +855,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="X16:Y16"/>
     <mergeCell ref="T16:U16"/>
     <mergeCell ref="V16:W16"/>
@@ -805,11 +867,6 @@
     <mergeCell ref="T14:U14"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B11:C11"/>
@@ -833,58 +890,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49944B09-6539-4790-B7BB-8FB56248F613}">
   <dimension ref="A2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="D4" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:C2"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:C3">
+    <cfRule type="notContainsErrors" dxfId="4" priority="1">
+      <formula>NOT(ISERROR(A3))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -893,51 +954,51 @@
   <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -945,6 +1006,11 @@
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:D3">
+    <cfRule type="notContainsErrors" dxfId="3" priority="1">
+      <formula>NOT(ISERROR(A3))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -953,51 +1019,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C2FF8C-FB76-489A-B0F1-EE2097262A74}">
   <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1005,7 +1071,13 @@
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:D3">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1014,51 +1086,58 @@
   <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:C3">
+    <cfRule type="notContainsErrors" dxfId="2" priority="1">
+      <formula>NOT(ISERROR(A3))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>